<commit_message>
MaJ Mockup + Modeles
</commit_message>
<xml_diff>
--- a/GestiBank - Modèles et Web Services.xlsx
+++ b/GestiBank - Modèles et Web Services.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="125">
   <si>
     <t>Nom</t>
   </si>
@@ -369,6 +369,27 @@
   </si>
   <si>
     <t>transactions</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>MessagePublic</t>
+  </si>
+  <si>
+    <t>MessageClient</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>sujet</t>
+  </si>
+  <si>
+    <t>Message  (classe abstraite)</t>
+  </si>
+  <si>
+    <t>titreCivilite</t>
   </si>
 </sst>
 </file>
@@ -844,7 +865,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -922,7 +943,7 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>37</v>
@@ -932,7 +953,7 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>37</v>
@@ -942,7 +963,7 @@
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>37</v>
@@ -952,7 +973,7 @@
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>37</v>
@@ -962,29 +983,25 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>36</v>
@@ -997,10 +1014,14 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>47</v>
@@ -1010,75 +1031,75 @@
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>37</v>
@@ -1088,229 +1109,225 @@
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="C27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>110</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
+      <c r="A41" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="C41" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>86</v>
@@ -1322,35 +1339,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>47</v>
@@ -1360,95 +1381,91 @@
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>108</v>
@@ -1462,73 +1479,121 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-    </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+      <c r="A57" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+      <c r="C58" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
+      <c r="C62" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -1540,7 +1605,7 @@
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -1552,7 +1617,7 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -1564,7 +1629,7 @@
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -1635,6 +1700,18 @@
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
MaJ WebSercice + Ajout DAO
</commit_message>
<xml_diff>
--- a/GestiBank - Modèles et Web Services.xlsx
+++ b/GestiBank - Modèles et Web Services.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Modèles" sheetId="2" r:id="rId1"/>
-    <sheet name="Web Services" sheetId="1" r:id="rId2"/>
+    <sheet name="DAO" sheetId="3" r:id="rId2"/>
+    <sheet name="Web Services" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="138">
   <si>
     <t>Nom</t>
   </si>
@@ -363,6 +364,72 @@
   </si>
   <si>
     <t>http://localhost:9090/GestiBankBackEnd</t>
+  </si>
+  <si>
+    <t>ConseillerController</t>
+  </si>
+  <si>
+    <t>findAllConseillers</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>/conseillers</t>
+  </si>
+  <si>
+    <t>/{id}</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>createConseiller</t>
+  </si>
+  <si>
+    <t>findConseillerById</t>
+  </si>
+  <si>
+    <t>deleteConseiller</t>
+  </si>
+  <si>
+    <t>updateConseiller</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Put</t>
+  </si>
+  <si>
+    <t>Objet Conseiller</t>
+  </si>
+  <si>
+    <t>Rechercher tous les conseillers</t>
+  </si>
+  <si>
+    <t>Recherche un conseiller avec son id</t>
+  </si>
+  <si>
+    <t>Créer un conseiller</t>
+  </si>
+  <si>
+    <t>Supprimer un conseiller</t>
+  </si>
+  <si>
+    <t>Mettre à jour un conseiller</t>
+  </si>
+  <si>
+    <t>GestiBank - DAO</t>
+  </si>
+  <si>
+    <t>DAO</t>
+  </si>
+  <si>
+    <t>ConseillerDAO</t>
+  </si>
+  <si>
+    <t>deleteConseillerById</t>
   </si>
 </sst>
 </file>
@@ -428,7 +495,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -514,12 +581,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -532,9 +610,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -552,6 +627,18 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -564,22 +651,34 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -909,946 +1008,946 @@
       <c r="D1" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="15"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="8" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="8" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="8" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="8" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="10" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="9" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="8" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="8" t="s">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="9" t="s">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="9" t="s">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="9" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="10" t="s">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="9" t="s">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="8" t="s">
+      <c r="C22" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="8" t="s">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="8" t="s">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="8" t="s">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="9" t="s">
+      <c r="C26" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="9" t="s">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="9" t="s">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="8" t="s">
+      <c r="C29" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="8" t="s">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="8" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="8" t="s">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="8" t="s">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="8" t="s">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="9" t="s">
+      <c r="C35" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="9" t="s">
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="8" t="s">
+      <c r="C37" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="7" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="8" t="s">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="7" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="9" t="s">
+      <c r="C39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="9" t="s">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="9" t="s">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="9" t="s">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E42" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="7" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D44" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="9" t="s">
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E46" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="9" t="s">
+      <c r="C47" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="9" t="s">
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E48" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="9" t="s">
+      <c r="A49" s="15"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="E49" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="9" t="s">
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E50" s="9" t="s">
+      <c r="E50" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D51" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="9" t="s">
+      <c r="D51" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D52" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="9" t="s">
+      <c r="D52" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="8" t="s">
+      <c r="C53" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="8" t="s">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E54" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="8" t="s">
+      <c r="A55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E55" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="11"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="8" t="s">
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E56" s="8" t="s">
+      <c r="E56" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="9" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C57" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D57" s="9" t="s">
+      <c r="D57" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E57" s="9" t="s">
+      <c r="E57" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
+      <c r="A58" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D58" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="9" t="s">
+      <c r="D58" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D59" s="9" t="s">
+      <c r="D59" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E59" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="8" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B60" s="8" t="s">
+      <c r="B60" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D60" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="9" t="s">
+      <c r="D60" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C61" s="9" t="s">
+      <c r="C61" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D61" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="9" t="s">
+      <c r="D61" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C62" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="D62" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="E62" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="8" t="s">
+      <c r="A63" s="17"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E63" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="9" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C64" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D64" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="8" t="s">
+      <c r="D64" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D65" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="8" t="s">
+      <c r="D65" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="12" t="s">
+      <c r="B66" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D66" s="9" t="s">
+      <c r="D66" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E66" s="9" t="s">
+      <c r="E66" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="9" t="s">
+      <c r="A67" s="15"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E67" s="9" t="s">
+      <c r="E67" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+      <c r="A68" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="11" t="s">
+      <c r="B68" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="D68" s="8" t="s">
+      <c r="D68" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="E68" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="11"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="8" t="s">
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E69" s="8" t="s">
+      <c r="E69" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="11"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="8" t="s">
+      <c r="A70" s="14"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="8" t="s">
+      <c r="E70" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="11"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="8" t="s">
+      <c r="A71" s="14"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="E71" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="9" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="C72" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D72" s="9" t="s">
+      <c r="D72" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E72" s="9" t="s">
+      <c r="E72" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1912,19 +2011,353 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="B3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.95" x14ac:dyDescent="0.25">
@@ -1937,128 +2370,194 @@
       <c r="E1" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="16" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="16" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="18"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="6" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="2"/>
+      <c r="A8" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="2"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="2"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="2"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="2"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2319,13 +2818,20 @@
       <c r="H39" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="13">
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>

</xml_diff>

<commit_message>
MaJ Suivi du projet
</commit_message>
<xml_diff>
--- a/GestiBank - Modèles et Web Services.xlsx
+++ b/GestiBank - Modèles et Web Services.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Adrien/Documents/Adrien/Travail/Global Knowledge/GestiBank/GestiBank-Divers/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{07C10621-40DE-1D47-8769-F0FB4CE04889}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16545" yWindow="465" windowWidth="12255" windowHeight="16395"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28760" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modèles" sheetId="2" r:id="rId1"/>
@@ -438,7 +444,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -642,9 +648,6 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -655,6 +658,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -748,7 +754,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -781,9 +787,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -816,6 +839,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -991,21 +1031,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -1013,18 +1053,18 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="15"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
@@ -1041,14 +1081,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1058,10 +1098,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="7" t="s">
         <v>57</v>
       </c>
@@ -1069,10 +1109,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="7" t="s">
         <v>18</v>
       </c>
@@ -1080,10 +1120,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="7" t="s">
         <v>100</v>
       </c>
@@ -1091,10 +1131,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="7" t="s">
         <v>102</v>
       </c>
@@ -1102,14 +1142,14 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -1119,10 +1159,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="9" t="s">
         <v>26</v>
       </c>
@@ -1130,10 +1170,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="8" t="s">
         <v>111</v>
       </c>
@@ -1141,14 +1181,14 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1158,10 +1198,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="7" t="s">
         <v>26</v>
       </c>
@@ -1169,10 +1209,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="7" t="s">
         <v>27</v>
       </c>
@@ -1180,14 +1220,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="8" t="s">
@@ -1197,10 +1237,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="8" t="s">
         <v>106</v>
       </c>
@@ -1208,10 +1248,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="8" t="s">
         <v>32</v>
       </c>
@@ -1219,10 +1259,10 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="8" t="s">
         <v>103</v>
       </c>
@@ -1230,10 +1270,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="9" t="s">
         <v>34</v>
       </c>
@@ -1241,10 +1281,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="8" t="s">
         <v>113</v>
       </c>
@@ -1252,14 +1292,14 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="7" t="s">
@@ -1269,10 +1309,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="7" t="s">
         <v>16</v>
       </c>
@@ -1280,10 +1320,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="7" t="s">
         <v>17</v>
       </c>
@@ -1291,10 +1331,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="7" t="s">
         <v>96</v>
       </c>
@@ -1302,14 +1342,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="8" t="s">
@@ -1319,10 +1359,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="8" t="s">
         <v>20</v>
       </c>
@@ -1330,10 +1370,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="8" t="s">
         <v>28</v>
       </c>
@@ -1341,14 +1381,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="7" t="s">
@@ -1358,10 +1398,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
       <c r="D30" s="7" t="s">
         <v>79</v>
       </c>
@@ -1369,10 +1409,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="7" t="s">
         <v>104</v>
       </c>
@@ -1380,10 +1420,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
       <c r="D32" s="7" t="s">
         <v>38</v>
       </c>
@@ -1391,10 +1431,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
       <c r="D33" s="7" t="s">
         <v>40</v>
       </c>
@@ -1402,10 +1442,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="7" t="s">
         <v>39</v>
       </c>
@@ -1413,14 +1453,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="8" t="s">
@@ -1430,10 +1470,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
       <c r="D36" s="8" t="s">
         <v>41</v>
       </c>
@@ -1441,14 +1481,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="7" t="s">
@@ -1458,10 +1498,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
       <c r="D38" s="7" t="s">
         <v>43</v>
       </c>
@@ -1469,14 +1509,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="8" t="s">
@@ -1486,10 +1526,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
       <c r="D40" s="8" t="s">
         <v>54</v>
       </c>
@@ -1497,10 +1537,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="8" t="s">
         <v>50</v>
       </c>
@@ -1508,10 +1548,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
       <c r="D42" s="8" t="s">
         <v>109</v>
       </c>
@@ -1519,7 +1559,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>82</v>
       </c>
@@ -1536,14 +1576,14 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="16" t="s">
         <v>44</v>
       </c>
       <c r="D44" s="8" t="s">
@@ -1553,10 +1593,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
       <c r="D45" s="8" t="s">
         <v>47</v>
       </c>
@@ -1564,7 +1604,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>85</v>
       </c>
@@ -1581,14 +1621,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="8" t="s">
@@ -1598,10 +1638,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="8" t="s">
         <v>91</v>
       </c>
@@ -1609,10 +1649,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
       <c r="D49" s="8" t="s">
         <v>92</v>
       </c>
@@ -1620,10 +1660,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
       <c r="D50" s="8" t="s">
         <v>93</v>
       </c>
@@ -1631,7 +1671,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>86</v>
       </c>
@@ -1648,7 +1688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>87</v>
       </c>
@@ -1665,14 +1705,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="C53" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D53" s="7" t="s">
@@ -1682,10 +1722,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
       <c r="D54" s="7" t="s">
         <v>53</v>
       </c>
@@ -1693,10 +1733,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
       <c r="D55" s="7" t="s">
         <v>60</v>
       </c>
@@ -1704,10 +1744,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="15"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
       <c r="D56" s="7" t="s">
         <v>54</v>
       </c>
@@ -1715,7 +1755,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
         <v>55</v>
       </c>
@@ -1732,7 +1772,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>64</v>
       </c>
@@ -1749,7 +1789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>95</v>
       </c>
@@ -1766,7 +1806,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>68</v>
       </c>
@@ -1783,7 +1823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>69</v>
       </c>
@@ -1800,14 +1840,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B62" s="18" t="s">
+      <c r="B62" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C62" s="18" t="s">
+      <c r="C62" s="17" t="s">
         <v>64</v>
       </c>
       <c r="D62" s="7" t="s">
@@ -1817,10 +1857,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="19"/>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="18"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
       <c r="D63" s="7" t="s">
         <v>66</v>
       </c>
@@ -1828,7 +1868,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>65</v>
       </c>
@@ -1845,7 +1885,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>110</v>
       </c>
@@ -1862,14 +1902,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="17" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C66" s="17" t="s">
+      <c r="C66" s="16" t="s">
         <v>51</v>
       </c>
       <c r="D66" s="8" t="s">
@@ -1879,10 +1919,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="17"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="16"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16"/>
       <c r="D67" s="8" t="s">
         <v>73</v>
       </c>
@@ -1890,14 +1930,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C68" s="16" t="s">
+      <c r="C68" s="15" t="s">
         <v>70</v>
       </c>
       <c r="D68" s="7" t="s">
@@ -1907,10 +1947,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="16"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="16"/>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="15"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="15"/>
       <c r="D69" s="7" t="s">
         <v>16</v>
       </c>
@@ -1918,10 +1958,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="16"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="15"/>
+      <c r="B70" s="15"/>
+      <c r="C70" s="15"/>
       <c r="D70" s="7" t="s">
         <v>17</v>
       </c>
@@ -1929,10 +1969,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="16"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="16"/>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="15"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="15"/>
       <c r="D71" s="7" t="s">
         <v>19</v>
       </c>
@@ -1940,7 +1980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
         <v>72</v>
       </c>
@@ -1959,12 +1999,38 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="C16:C21"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="C47:C50"/>
     <mergeCell ref="A53:A56"/>
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="C53:C56"/>
@@ -1977,38 +2043,12 @@
     <mergeCell ref="A62:A63"/>
     <mergeCell ref="B62:B63"/>
     <mergeCell ref="C62:C63"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B16:B21"/>
-    <mergeCell ref="C16:C21"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2016,21 +2056,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>134</v>
       </c>
@@ -2039,19 +2079,19 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="19"/>
       <c r="B4" s="13" t="s">
         <v>0</v>
       </c>
@@ -2065,7 +2105,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>136</v>
       </c>
@@ -2082,7 +2122,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
       <c r="B6" s="12" t="s">
         <v>123</v>
@@ -2097,7 +2137,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
       <c r="B7" s="12" t="s">
         <v>122</v>
@@ -2112,7 +2152,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="B8" s="12" t="s">
         <v>124</v>
@@ -2127,7 +2167,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="22"/>
       <c r="B9" s="20" t="s">
         <v>125</v>
@@ -2142,7 +2182,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="22"/>
       <c r="B10" s="21"/>
       <c r="C10" s="12" t="s">
@@ -2151,182 +2191,182 @@
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2347,24 +2387,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.95" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -2373,7 +2413,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>12</v>
       </c>
@@ -2383,7 +2423,7 @@
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>4</v>
       </c>
@@ -2397,7 +2437,7 @@
       <c r="G5" s="26"/>
       <c r="H5" s="27"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
         <v>0</v>
       </c>
@@ -2413,7 +2453,7 @@
       <c r="G6" s="26"/>
       <c r="H6" s="27"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="29"/>
       <c r="B7" s="29"/>
       <c r="C7" s="11" t="s">
@@ -2435,7 +2475,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>116</v>
       </c>
@@ -2461,7 +2501,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
       <c r="C9" s="12" t="s">
@@ -2483,7 +2523,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
       <c r="C10" s="12" t="s">
@@ -2505,7 +2545,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
       <c r="C11" s="12" t="s">
@@ -2527,7 +2567,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="23"/>
       <c r="B12" s="23"/>
       <c r="C12" s="20" t="s">
@@ -2545,11 +2585,11 @@
       <c r="G12" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
       <c r="C13" s="21"/>
@@ -2559,9 +2599,9 @@
       <c r="G13" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2838,7 +2878,7 @@
     <mergeCell ref="B6:B7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>